<commit_message>
standardised arbitrary stimuli to those used by Leader and Barnes-Holmes’s (2001b)
</commit_message>
<xml_diff>
--- a/stimuli ALT - ARBITRARY.xlsx
+++ b/stimuli ALT - ARBITRARY.xlsx
@@ -30,27 +30,6 @@
     <t>VEK</t>
   </si>
   <si>
-    <t>PIM</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>BRU</t>
-  </si>
-  <si>
-    <t>IKA</t>
-  </si>
-  <si>
-    <t>NAR</t>
-  </si>
-  <si>
-    <t>TIV</t>
-  </si>
-  <si>
-    <t>ORT</t>
-  </si>
-  <si>
     <t>a1_exemplar</t>
   </si>
   <si>
@@ -80,12 +59,33 @@
   <si>
     <t>mastery_criterion</t>
   </si>
+  <si>
+    <t>ZID</t>
+  </si>
+  <si>
+    <t>YIM</t>
+  </si>
+  <si>
+    <t>PAF</t>
+  </si>
+  <si>
+    <t>ROG</t>
+  </si>
+  <si>
+    <t>MAU</t>
+  </si>
+  <si>
+    <t>JOM</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -101,6 +101,10 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="LiberationSerif"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,7 +124,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="739">
+  <cellStyleXfs count="743">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -860,13 +864,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="739">
+  <cellStyles count="743">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1236,6 +1245,8 @@
     <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1605,6 +1616,8 @@
     <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1932,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1948,34 +1961,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="J1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1983,32 +1996,35 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <v>15</v>
       </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>